<commit_message>
feat : jpa-study * codes typed learning JPA course
</commit_message>
<xml_diff>
--- a/prj-01-LMS/학습관리사이트분석.xlsx
+++ b/prj-01-LMS/학습관리사이트분석.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sebinSample\spring\prj-01-LMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70882E69-6C9E-4600-AF48-E6DE6C1137AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8585D4A6-4C70-4BB7-BC3F-929EAB222F73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="705" yWindow="2085" windowWidth="24900" windowHeight="13515" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="1305" windowWidth="12420" windowHeight="13515" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -313,26 +313,26 @@
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -616,8 +616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -631,8 +631,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
     </row>
     <row r="2" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
@@ -641,194 +641,194 @@
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="3"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="2"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="4" t="s">
+      <c r="E3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="3"/>
+      <c r="G3" s="2"/>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="7" t="s">
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="5" t="s">
+      <c r="E4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="4"/>
+      <c r="G4" s="3"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="7" t="s">
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="3" t="s">
+      <c r="E5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="3"/>
+      <c r="G5" s="2"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="7" t="s">
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="3"/>
+      <c r="G6" s="2"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="7" t="s">
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B8" s="8"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="7" t="s">
+      <c r="B8" s="9"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="8"/>
-      <c r="C9" s="6" t="s">
+      <c r="B9" s="9"/>
+      <c r="C9" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="7" t="s">
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="7" t="s">
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="7" t="s">
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="10" t="s">
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="7" t="s">
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="7" t="s">
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="5" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="7" t="s">
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E16" s="5" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B17" s="8"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="7" t="s">
+      <c r="B17" s="9"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E17" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B18" s="8"/>
-      <c r="C18" s="6" t="s">
+      <c r="B18" s="9"/>
+      <c r="C18" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E18" s="5" t="s">
         <v>8</v>
       </c>
       <c r="F18" t="s">
@@ -836,12 +836,12 @@
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="7" t="s">
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E19" s="5" t="s">
         <v>8</v>
       </c>
       <c r="F19" t="s">
@@ -849,12 +849,12 @@
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="7" t="s">
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="E20" s="5" t="s">
         <v>8</v>
       </c>
       <c r="F20" t="s">
@@ -862,54 +862,54 @@
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B21" s="8"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="7" t="s">
+      <c r="B21" s="9"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="E21" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B22" s="8"/>
-      <c r="C22" s="6" t="s">
+      <c r="B22" s="9"/>
+      <c r="C22" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E22" s="7" t="s">
+      <c r="E22" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="7" t="s">
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="E23" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="7" t="s">
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E24" s="7" t="s">
+      <c r="E24" s="5" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B25" s="9"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="7" t="s">
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E25" s="7" t="s">
+      <c r="E25" s="5" t="s">
         <v>8</v>
       </c>
       <c r="F25" t="s">
@@ -918,12 +918,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="B3:B25"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="C22:C25"/>
     <mergeCell ref="C18:C21"/>
     <mergeCell ref="C9:C17"/>
     <mergeCell ref="C3:C8"/>
-    <mergeCell ref="B3:B25"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>